<commit_message>
tests: updated tests to check for validity of the length and indel placement in the reference parsing
</commit_message>
<xml_diff>
--- a/extract_indels/test_data/test_all_indels_list_ref.xlsx
+++ b/extract_indels/test_data/test_all_indels_list_ref.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac_studio_np/Documents/bin/reusable_small_scripts/extract_indels/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94964AAF-DABD-7B42-83EF-E16F6FD58A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5331CE7F-2D2B-5146-8832-37175357882B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1500" windowWidth="34100" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="500" windowWidth="34100" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_all_indels" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test_all_indels!$A$1:$T$544</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test_all_indels!$A$1:$U$544</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3278" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3281" uniqueCount="182">
   <si>
     <t>#CHROM</t>
   </si>
@@ -573,6 +573,15 @@
   </si>
   <si>
     <t>STRND_BIAS_PASS</t>
+  </si>
+  <si>
+    <t>PLACEMENT</t>
+  </si>
+  <si>
+    <t>CTAGGGAGAGCTGCC*TA*TATGGAAGAGCCCTA</t>
+  </si>
+  <si>
+    <t>TTACTTGGTTCCATG*CTATACATGTCTCTGGGACCAATGGTA*CTAAGAGGTTTGATA</t>
   </si>
 </sst>
 </file>
@@ -1469,19 +1478,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T544"/>
+  <dimension ref="A1:U544"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A519" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R533" sqref="R533"/>
+      <selection pane="bottomLeft" activeCell="U538" sqref="U538"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="20" max="20" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" hidden="1" customWidth="1"/>
+    <col min="14" max="17" width="0.1640625" hidden="1" customWidth="1"/>
+    <col min="18" max="20" width="0.1640625" customWidth="1"/>
+    <col min="21" max="21" width="67.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1542,8 +1556,11 @@
       <c r="T1" s="3" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U1" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1607,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1671,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1735,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1799,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1863,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1927,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1991,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2055,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2119,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2183,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2247,7 +2264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -2311,7 +2328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -2375,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -2439,7 +2456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -27079,7 +27096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>7</v>
       </c>
@@ -27143,7 +27160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>7</v>
       </c>
@@ -27207,7 +27224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>7</v>
       </c>
@@ -27271,7 +27288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>7</v>
       </c>
@@ -27335,7 +27352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>7</v>
       </c>
@@ -27399,7 +27416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>7</v>
       </c>
@@ -27463,7 +27480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>7</v>
       </c>
@@ -27527,7 +27544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="408" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>7</v>
       </c>
@@ -27591,7 +27608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>7</v>
       </c>
@@ -27655,7 +27672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A410" s="4" t="s">
         <v>7</v>
       </c>
@@ -27718,8 +27735,11 @@
       <c r="T410" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="411" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U410" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="411" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>7</v>
       </c>
@@ -27783,7 +27803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>7</v>
       </c>
@@ -27847,7 +27867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>7</v>
       </c>
@@ -27911,7 +27931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>7</v>
       </c>
@@ -27975,7 +27995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>7</v>
       </c>
@@ -28039,7 +28059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>7</v>
       </c>
@@ -35271,7 +35291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="529" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>7</v>
       </c>
@@ -35335,7 +35355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="530" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A530" t="s">
         <v>7</v>
       </c>
@@ -35399,7 +35419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="531" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
         <v>7</v>
       </c>
@@ -35463,7 +35483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="532" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
         <v>7</v>
       </c>
@@ -35527,7 +35547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="533" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
         <v>7</v>
       </c>
@@ -35591,7 +35611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="534" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A534" t="s">
         <v>7</v>
       </c>
@@ -35655,7 +35675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="535" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
         <v>7</v>
       </c>
@@ -35719,7 +35739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="536" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
         <v>7</v>
       </c>
@@ -35783,7 +35803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="537" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A537" t="s">
         <v>7</v>
       </c>
@@ -35847,7 +35867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="538" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A538" s="4" t="s">
         <v>7</v>
       </c>
@@ -35910,8 +35930,11 @@
       <c r="T538" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="539" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U538" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="539" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
         <v>7</v>
       </c>
@@ -35975,7 +35998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="540" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>7</v>
       </c>
@@ -36039,7 +36062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="541" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="541" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A541" t="s">
         <v>7</v>
       </c>
@@ -36103,7 +36126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="542" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>7</v>
       </c>
@@ -36167,7 +36190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="543" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
         <v>7</v>
       </c>
@@ -36231,7 +36254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="544" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
         <v>7</v>
       </c>
@@ -36296,12 +36319,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T544" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:U544" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="T1:T1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>